<commit_message>
added topic 3 breakout activity answer
</commit_message>
<xml_diff>
--- a/public/slides/03-slide/Breakout Assignment Student Copy.xlsx
+++ b/public/slides/03-slide/Breakout Assignment Student Copy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Dong\Dropbox\Work\Gooder\PhD\TA\MBAS 821\Shared files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Dong\Dropbox\Work\Gooder\PhD\Website\web1\static\slides\03-slide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E54BA72A-E0D7-4F59-9256-C75176045620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4A2134-FBA0-43F5-8747-0DF2D5624DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,13 +161,13 @@
     <t>CCA Tax shield</t>
   </si>
   <si>
-    <t>OCF [(3) + (5)]</t>
-  </si>
-  <si>
     <t>(12)</t>
   </si>
   <si>
     <t>FCF [(6) + (11)]</t>
+  </si>
+  <si>
+    <t>OCF [(3) x (1-Tc) + (5)]</t>
   </si>
 </sst>
 </file>
@@ -182,8 +182,8 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;0&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;0&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -359,7 +359,7 @@
     </xf>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -380,22 +380,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -681,7 +681,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -807,7 +807,7 @@
       <c r="B5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -846,8 +846,8 @@
       <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="9" t="s">
         <v>9</v>
       </c>
@@ -924,9 +924,9 @@
         <v>17</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
@@ -947,9 +947,9 @@
         <v>37</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
@@ -966,13 +966,13 @@
       <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
@@ -993,9 +993,9 @@
         <v>40</v>
       </c>
       <c r="C13" s="32"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
@@ -1013,12 +1013,12 @@
         <v>21</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C14" s="32"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -1216,10 +1216,10 @@
       <c r="B23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
@@ -1295,15 +1295,15 @@
     </row>
     <row r="27" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
@@ -1317,8 +1317,8 @@
       <c r="Q27" s="20"/>
     </row>
     <row r="28" spans="1:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="35"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1381,8 +1381,8 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
       <c r="D31" s="22"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
@@ -1400,8 +1400,8 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="38"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="35"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
@@ -1419,8 +1419,8 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
@@ -1438,8 +1438,8 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="20"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="38"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>

</xml_diff>